<commit_message>
fixed an error - C# and C++ were not showing up..
</commit_message>
<xml_diff>
--- a/languagedata.xlsx
+++ b/languagedata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>rails</t>
   </si>
@@ -181,6 +181,18 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>c++</t>
+  </si>
+  <si>
+    <t>.net</t>
+  </si>
+  <si>
+    <t>c#</t>
+  </si>
+  <si>
+    <t>asp.net</t>
   </si>
 </sst>
 </file>
@@ -277,166 +289,166 @@
               <c:strCache>
                 <c:ptCount val="54"/>
                 <c:pt idx="0">
+                  <c:v>sql</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>java</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>xml</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>microsoft</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>linux</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>office</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>c++</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>c</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>sql</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>java</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>xml</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>microsoft</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>linux</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>office</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>unix</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>oracle</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>html</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>javascript</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>perl</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>python</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
+                  <c:v>.net</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>nosql</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
+                  <c:v>c#</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>flash</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>photoshop</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
+                  <c:v>ajax</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>adobe</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>mysql</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>ajax</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>adobe</c:v>
-                </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>vpn</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>android</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="24">
                   <c:v>php</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="25">
                   <c:v>ios</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="26">
+                  <c:v>verilog</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>matlab</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>verilog</c:v>
-                </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="28">
+                  <c:v>rest</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>asp.net</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>dns</c:v>
                 </c:pt>
-                <c:pt idx="26">
-                  <c:v>rest</c:v>
-                </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="31">
                   <c:v>sdlc</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="32">
                   <c:v>soap</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="33">
                   <c:v>ruby</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="34">
                   <c:v>ipsec</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="35">
+                  <c:v>hibernate</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>schema</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>mongodb</c:v>
                 </c:pt>
-                <c:pt idx="32">
-                  <c:v>hibernate</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>schema</c:v>
-                </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="38">
                   <c:v>dreamweaver</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="39">
                   <c:v>batch</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="40">
+                  <c:v>gsm</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>scala</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>cdma</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>ood</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>struts</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>vb</c:v>
                 </c:pt>
-                <c:pt idx="37">
-                  <c:v>gsm</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>scala</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>struts</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>cdma</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>ood</c:v>
-                </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="46">
+                  <c:v>lte</c:v>
+                </c:pt>
+                <c:pt idx="47">
                   <c:v>jsp</c:v>
                 </c:pt>
-                <c:pt idx="43">
-                  <c:v>lte</c:v>
-                </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="48">
                   <c:v>lamp</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="49">
                   <c:v>django</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="50">
                   <c:v>vbscript</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="51">
+                  <c:v>fortran</c:v>
+                </c:pt>
+                <c:pt idx="52">
                   <c:v>vba</c:v>
                 </c:pt>
-                <c:pt idx="48">
-                  <c:v>fortran</c:v>
-                </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="53">
                   <c:v>wlan</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>swing</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>wwan</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>prolog</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>rails</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -448,166 +460,166 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="54"/>
                 <c:pt idx="0">
-                  <c:v>430.0</c:v>
+                  <c:v>354.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>360.0</c:v>
+                  <c:v>331.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>342.0</c:v>
+                  <c:v>277.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>277.0</c:v>
+                  <c:v>219.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>222.0</c:v>
+                  <c:v>212.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>215.0</c:v>
+                  <c:v>204.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>213.0</c:v>
+                  <c:v>167.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>146.0</c:v>
+                  <c:v>158.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>136.0</c:v>
+                  <c:v>145.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>135.0</c:v>
+                  <c:v>130.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100.0</c:v>
+                  <c:v>124.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>95.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>92.0</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>90.0</c:v>
-                </c:pt>
                 <c:pt idx="13">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>65.0</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>57.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>56.0</c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>49.0</c:v>
+                  <c:v>64.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>48.0</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>47.0</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>44.0</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>43.0</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>41.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="24">
                   <c:v>40.0</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="25">
                   <c:v>39.0</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="26">
                   <c:v>36.0</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="27">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>34.0</c:v>
                 </c:pt>
-                <c:pt idx="26">
-                  <c:v>34.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>27.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>25.0</c:v>
-                </c:pt>
                 <c:pt idx="29">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="33">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>20.0</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="35">
                   <c:v>20.0</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="36">
                   <c:v>20.0</c:v>
                 </c:pt>
-                <c:pt idx="33">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
                   <c:v>13.0</c:v>
                 </c:pt>
-                <c:pt idx="36">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="40">
                   <c:v>11.0</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="41">
                   <c:v>11.0</c:v>
                 </c:pt>
-                <c:pt idx="39">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="42">
                   <c:v>10.0</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="43">
                   <c:v>10.0</c:v>
                 </c:pt>
-                <c:pt idx="42">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="44">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>7.0</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="47">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
                   <c:v>5.0</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="49">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="50">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="51">
                   <c:v>3.0</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="52">
                   <c:v>3.0</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="53">
                   <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -622,11 +634,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2131396376"/>
-        <c:axId val="2091638872"/>
+        <c:axId val="2144808104"/>
+        <c:axId val="2144813512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2131396376"/>
+        <c:axId val="2144808104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -654,7 +666,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2091638872"/>
+        <c:crossAx val="2144813512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -662,7 +674,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2091638872"/>
+        <c:axId val="2144813512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -692,7 +704,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2131396376"/>
+        <c:crossAx val="2144808104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1066,443 +1078,475 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1">
-        <v>430</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2">
-        <v>360</v>
+        <v>331</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3">
-        <v>342</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4">
-        <v>277</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B7">
-        <v>213</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B8">
-        <v>146</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9">
-        <v>136</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B11">
-        <v>100</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B12">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B14">
-        <v>65</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B15">
-        <v>57</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B16">
-        <v>56</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="B17">
-        <v>49</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B18">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B19">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B20">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B21">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B22">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B23">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B24">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B25">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B26">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B27">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B28">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B30">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B31">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B32">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B33">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B34">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B35">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B36">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B37">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B38">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B39">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B40">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B41">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B42">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B43">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44">
         <v>10</v>
-      </c>
-      <c r="B44">
-        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B45">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46">
         <v>8</v>
-      </c>
-      <c r="B46">
-        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47">
         <v>7</v>
-      </c>
-      <c r="B47">
-        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B48">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49">
         <v>5</v>
-      </c>
-      <c r="B49">
-        <v>3</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50">
         <v>4</v>
-      </c>
-      <c r="B50">
-        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B51">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B52">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
         <v>0</v>
       </c>
-      <c r="B54">
+      <c r="B58">
         <v>1</v>
       </c>
     </row>

</xml_diff>